<commit_message>
Update project structure and documentation
</commit_message>
<xml_diff>
--- a/docs/太极电脑管家纳管业务流程基本功能点.xlsx
+++ b/docs/太极电脑管家纳管业务流程基本功能点.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>服务端功能</t>
   </si>
@@ -74,10 +74,25 @@
     <t>显示注册终端信息，支持对终端按照SN、用户、IP、MAC等信息查找和筛选。</t>
   </si>
   <si>
+    <t>通过</t>
+  </si>
+  <si>
     <t>分组管理</t>
   </si>
   <si>
-    <t>用户自定义逻辑分组，可创建、编辑、删除分组。订单导入后自动创建库存分组，订单中SN自动保存在库存中。</t>
+    <r>
+      <t>用户自定义逻辑分组，可创建、编辑、删除分组。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>订单导入后自动创建库存分组，订单中SN自动保存在库存中。</t>
+    </r>
   </si>
   <si>
     <t>批量编辑资产信息</t>
@@ -95,7 +110,29 @@
     <t>终端注销</t>
   </si>
   <si>
-    <t>注销终端，注销后终端回到库存分组，并不在接收上报数据</t>
+    <r>
+      <t>注销终端，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>注销后终端回到库存分组</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，并不在接收上报数据</t>
+    </r>
   </si>
   <si>
     <t>生成报表</t>
@@ -104,10 +141,31 @@
     <t>生成资产报告，可自定义字段</t>
   </si>
   <si>
+    <t>未通过</t>
+  </si>
+  <si>
+    <t>能生成资产报告、但是不可以自定义字段</t>
+  </si>
+  <si>
     <t>用户管理</t>
   </si>
   <si>
-    <t>支持导入和批量创建用户。用户和资产通过SN号进行绑定或解绑</t>
+    <r>
+      <t>支持导入和批量创建用户。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>用户和资产通过SN号进行绑定或解绑</t>
+    </r>
+  </si>
+  <si>
+    <t>能批量导入和批量创建用户，但是不能批量通过SN进行绑定，只能导入一个SN</t>
   </si>
   <si>
     <t>健康监测</t>
@@ -119,6 +177,9 @@
     <t>对终端硬件如CPU使用率，内存使用率，硬盘使用率，CPU温度，终端使用频次。阈值可设置</t>
   </si>
   <si>
+    <t>没找到该功能</t>
+  </si>
+  <si>
     <t>告警提示</t>
   </si>
   <si>
@@ -174,6 +235,9 @@
   </si>
   <si>
     <t>Server端发起注销流程。注销后设备回到库存中，server不对设备进行管控</t>
+  </si>
+  <si>
+    <t>注销后设备未回到库存中</t>
   </si>
   <si>
     <t>设备信息采集</t>
@@ -210,7 +274,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,8 +440,15 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,6 +458,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -724,7 +801,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -748,16 +825,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -766,89 +843,89 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -873,13 +950,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1198,14 +1278,14 @@
   <sheetPr/>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="13.5533333333333" style="3" customWidth="1"/>
-    <col min="2" max="2" width="21" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.1" style="3" customWidth="1"/>
     <col min="3" max="3" width="95" style="3" customWidth="1"/>
     <col min="4" max="4" width="9.66666666666667" style="3" customWidth="1"/>
     <col min="5" max="5" width="55" style="3" customWidth="1"/>
@@ -1245,7 +1325,7 @@
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="7"/>
@@ -1256,11 +1336,11 @@
       <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="9"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" ht="16.5" spans="1:5">
       <c r="A5" s="6" t="s">
@@ -1272,160 +1352,190 @@
       <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" ht="16.5" spans="1:5">
       <c r="A6" s="6"/>
       <c r="B6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
     <row r="7" ht="16.5" spans="1:5">
       <c r="A7" s="6"/>
       <c r="B7" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" ht="16.5" spans="1:5">
       <c r="A8" s="6"/>
       <c r="B8" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E8" s="7"/>
     </row>
     <row r="9" ht="16.5" spans="1:5">
       <c r="A9" s="6"/>
       <c r="B9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="C9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E9" s="7"/>
     </row>
     <row r="10" ht="16.5" spans="1:5">
       <c r="A10" s="6"/>
       <c r="B10" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" ht="16.5" spans="1:5">
       <c r="A11" s="6"/>
       <c r="B11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" ht="16.5" spans="1:5">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" ht="16.5" spans="1:5">
       <c r="A13" s="6"/>
       <c r="B13" s="7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E13" s="7"/>
     </row>
     <row r="14" ht="16.5" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="7"/>
+        <v>38</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E14" s="7"/>
     </row>
     <row r="15" ht="16.5" spans="1:5">
       <c r="A15" s="6"/>
       <c r="B15" s="7" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="10"/>
+        <v>40</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" ht="33" spans="1:5">
-      <c r="A16" s="7" t="s">
-        <v>36</v>
+      <c r="A16" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E16" s="7"/>
     </row>
     <row r="17" customFormat="1" spans="1:5">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" customFormat="1" spans="1:5">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" s="2" customFormat="1" spans="1:5">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="11"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1451,91 +1561,101 @@
     </row>
     <row r="22" ht="16.5" spans="1:5">
       <c r="A22" s="7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
     <row r="23" ht="33" spans="1:5">
       <c r="A23" s="7" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="7"/>
+        <v>49</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E23" s="7"/>
     </row>
     <row r="24" ht="16.5" spans="1:5">
       <c r="A24" s="7" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+        <v>52</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="25" ht="16.5" spans="1:5">
       <c r="A25" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="7"/>
+        <v>55</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E25" s="7"/>
     </row>
     <row r="26" ht="16.5" spans="1:5">
       <c r="A26" s="7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="7"/>
+        <v>57</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E26" s="7"/>
     </row>
     <row r="27" ht="16.5" spans="1:5">
       <c r="A27" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>52</v>
+        <v>58</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D27" s="7"/>
-      <c r="E27" s="10"/>
+      <c r="E27" s="9"/>
     </row>
     <row r="28" ht="16.5" spans="1:5">
       <c r="A28" s="7" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>

</xml_diff>